<commit_message>
replace RTMF with NV version (less shift to rail)
</commit_message>
<xml_diff>
--- a/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
+++ b/InputData/trans/RTMF/Recipient Transportation Mode Fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/trans/rtmf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Nevada\NV_model\InputData\trans\RTMF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114B00CC-B2D0-544D-9B60-1EEAFB4C53B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7159C0C3-3BCF-4B40-A1A8-AC29F16AE72E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="2260" windowWidth="23600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4365" yWindow="600" windowWidth="24435" windowHeight="15630" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -216,7 +216,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,22 +532,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7">
-        <v>44307</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -556,80 +552,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>24</v>
@@ -638,7 +634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>25</v>
@@ -647,7 +643,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -669,16 +665,18 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -704,7 +702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -712,13 +710,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="4">
-        <v>0.33</v>
+        <v>0.15</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>0.33</v>
+        <v>0.05</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
@@ -728,11 +726,10 @@
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="6">
-        <f>1-SUM(B2:G2)</f>
-        <v>0.33999999999999997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -760,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -788,7 +785,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -816,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -844,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -872,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -893,18 +890,18 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -930,7 +927,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -958,7 +955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -986,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1042,7 +1039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1098,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>

</xml_diff>